<commit_message>
add naive unit options for parsers, #778
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-pit tagging.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-pit tagging.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>Vial Number</t>
   </si>
@@ -102,7 +102,16 @@
     <t>2021 FP</t>
   </si>
   <si>
-    <t>Column1</t>
+    <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>Length (mm)</t>
+  </si>
+  <si>
+    <t>922222220125</t>
+  </si>
+  <si>
+    <t>922222220124</t>
   </si>
 </sst>
 </file>
@@ -161,12 +170,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,22 +473,26 @@
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -487,10 +505,10 @@
       <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -512,15 +530,21 @@
         <v>8</v>
       </c>
       <c r="M3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -532,10 +556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:P5"/>
+  <dimension ref="A3:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,21 +568,23 @@
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -578,37 +604,43 @@
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -621,41 +653,41 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>922222220124</v>
-      </c>
-      <c r="F4">
-        <v>922222220124</v>
-      </c>
-      <c r="G4">
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4">
         <v>30.5</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>332</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>23</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>19</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>20</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>21</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -668,37 +700,37 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>922222220125</v>
-      </c>
-      <c r="F5">
-        <v>922222220125</v>
-      </c>
-      <c r="G5">
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5">
         <v>30.5</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>332</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>23</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>18</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>19</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>20</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>21</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add tests for movement fix, #824
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-pit tagging.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-pit tagging.xlsx
@@ -119,6 +119,32 @@
           </rPr>
           <t xml:space="preserve">
 eg: 1999 FP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fill in to record current container, or if movement occurred.  Leave blank if movement origin is unknown.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fill in if a movement occurred, or if origin tank is unknown.</t>
         </r>
       </text>
     </comment>
@@ -278,7 +304,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +314,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,6 +355,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,7 +639,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="K3" sqref="K3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,10 +698,10 @@
       <c r="J3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="M3" s="2" t="s">

</xml_diff>